<commit_message>
updated code to plot charts in new sheet
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
-  <si>
-    <t>date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>Items</t>
@@ -49,6 +50,21 @@
     <t>01/07/2023</t>
   </si>
   <si>
+    <t>01/08/2023</t>
+  </si>
+  <si>
+    <t>01/09/2023</t>
+  </si>
+  <si>
+    <t>01/10/2023</t>
+  </si>
+  <si>
+    <t>01/11/2023</t>
+  </si>
+  <si>
+    <t>01/12/2023</t>
+  </si>
+  <si>
     <t>Bookcase</t>
   </si>
   <si>
@@ -62,6 +78,27 @@
   </si>
   <si>
     <t>Frame</t>
+  </si>
+  <si>
+    <t>Vase</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Lamp</t>
+  </si>
+  <si>
+    <t>TV Console</t>
+  </si>
+  <si>
+    <t>Blinds</t>
+  </si>
+  <si>
+    <t>Curtain</t>
+  </si>
+  <si>
+    <t>Shelf</t>
   </si>
   <si>
     <t>FURNITURE STORE SALES REPORT</t>
@@ -117,7 +154,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -182,7 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <border>
         <left style="medium">
@@ -222,9 +259,481 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00_);(#,##0.00)"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="dd-mmm-yyyy"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="10"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Profit by Items</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Profit</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$C$5:$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bookcase</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Table</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Art</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Frame</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Vase</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lamp</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TV Console</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Blinds</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Curtain</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Shelf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$F$5:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Items</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Profit (NGN)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Profit by Items</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sales</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$5:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>01/01/2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01/02/2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01/03/2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>01/04/2023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>01/05/2023</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>01/06/2023</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>01/07/2023</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>01/08/2023</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>01/09/2023</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>01/10/2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>01/11/2023</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01/12/2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18570</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14650</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Items</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Profit (NGN)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,15 +1021,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -530,7 +1042,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -552,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -563,7 +1075,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>15000</v>
@@ -584,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>12500</v>
@@ -605,7 +1117,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>10000</v>
@@ -626,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>4000</v>
@@ -644,10 +1156,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>2500</v>
@@ -665,10 +1177,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>13500</v>
@@ -686,10 +1198,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>12000</v>
@@ -707,10 +1219,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>15000</v>
@@ -728,10 +1240,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>12500</v>
@@ -749,10 +1261,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>10000</v>
@@ -770,10 +1282,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>4000</v>
@@ -791,10 +1303,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>2500</v>
@@ -807,58 +1319,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <v>13500</v>
-      </c>
-      <c r="E17">
-        <v>19500</v>
-      </c>
-      <c r="F17" s="5">
-        <f>E17-D17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="3">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>12000</v>
-      </c>
-      <c r="E18">
-        <v>14350</v>
-      </c>
-      <c r="F18" s="5">
-        <f>E18-D18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="C19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="7">
-        <f>SUM(E5:E18)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <f>SUM(F5:F18)</f>
+    <row r="17" spans="3:6">
+      <c r="C17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7">
+        <f>SUM(E5:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <f>SUM(F5:F16)</f>
         <v>0</v>
       </c>
     </row>
@@ -875,7 +1345,7 @@
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:F19">
+  <conditionalFormatting sqref="A5:F17">
     <cfRule type="notContainsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
@@ -883,11 +1353,29 @@
       <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:E19">
+  <conditionalFormatting sqref="B5:B17">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="6">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:E17">
     <cfRule type="notContainsBlanks" dxfId="2" priority="5">
       <formula>LEN(TRIM(D5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update sales report index
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -47,24 +47,6 @@
     <t>01/06/2023</t>
   </si>
   <si>
-    <t>01/07/2023</t>
-  </si>
-  <si>
-    <t>01/08/2023</t>
-  </si>
-  <si>
-    <t>01/09/2023</t>
-  </si>
-  <si>
-    <t>01/10/2023</t>
-  </si>
-  <si>
-    <t>01/11/2023</t>
-  </si>
-  <si>
-    <t>01/12/2023</t>
-  </si>
-  <si>
     <t>Bookcase</t>
   </si>
   <si>
@@ -72,30 +54,6 @@
   </si>
   <si>
     <t>Table</t>
-  </si>
-  <si>
-    <t>Art</t>
-  </si>
-  <si>
-    <t>Frame</t>
-  </si>
-  <si>
-    <t>Vase</t>
-  </si>
-  <si>
-    <t>Fan</t>
-  </si>
-  <si>
-    <t>Lamp</t>
-  </si>
-  <si>
-    <t>TV Console</t>
-  </si>
-  <si>
-    <t>Blinds</t>
-  </si>
-  <si>
-    <t>Curtain</t>
   </si>
   <si>
     <t>Shelf</t>
@@ -131,7 +89,7 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,7 +97,7 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -198,10 +162,10 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -283,7 +247,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Profit by Items</a:t>
+              <a:t>Cost and Sales Price by Item</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -299,13 +263,21 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Profit</c:v>
+            <c:strRef>
+              <c:f>Chart!B4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sales!$C$5:$C$16</c:f>
+              <c:f>Chart!$A$5:$A8</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Bookcase</c:v>
                 </c:pt>
@@ -313,79 +285,87 @@
                   <c:v>Chair</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Shelf</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Table</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Art</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Frame</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Vase</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Fan</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Lamp</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>TV Console</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Blinds</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Curtain</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Shelf</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sales!$F$5:$F$16</c:f>
+              <c:f>Chart!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>19000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!C4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sale Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$5:$A8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bookcase</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shelf</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Table</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -442,7 +422,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Profit (NGN)</a:t>
+                  <a:t>Price (NGN)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -452,207 +432,6 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Profit by Items</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Sales</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sales!$B$5:$B$16</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>01/01/2023</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>01/02/2023</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>01/03/2023</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>01/04/2023</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>01/05/2023</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>01/06/2023</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>01/07/2023</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>01/08/2023</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>01/09/2023</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>01/10/2023</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>01/11/2023</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>01/12/2023</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sales!$E$5:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>18000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4550</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18570</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14650</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15450</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17800</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6900</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4950</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50020001"/>
-        <c:axId val="50020002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50020001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Items</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50020002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Profit (NGN)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -675,13 +454,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -698,36 +477,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1032,7 +781,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1042,7 +791,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1064,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1075,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>15000</v>
@@ -1093,10 +842,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>12500</v>
@@ -1114,10 +863,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>10000</v>
@@ -1135,10 +884,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>4000</v>
@@ -1156,10 +905,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>2500</v>
@@ -1177,10 +926,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>13500</v>
@@ -1198,10 +947,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>12000</v>
@@ -1219,10 +968,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>15000</v>
@@ -1240,10 +989,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>12500</v>
@@ -1261,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>10000</v>
@@ -1282,10 +1031,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>4000</v>
@@ -1303,10 +1052,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D16">
         <v>2500</v>
@@ -1321,7 +1070,11 @@
     </row>
     <row r="17" spans="3:6">
       <c r="C17" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="D17" s="7">
+        <f>SUM(D5:D16)</f>
+        <v>0</v>
       </c>
       <c r="E17" s="7">
         <f>SUM(E5:E16)</f>
@@ -1369,12 +1122,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>19000</v>
+      </c>
+      <c r="C5">
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>31500</v>
+      </c>
+      <c r="C6">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>27000</v>
+      </c>
+      <c r="C7">
+        <v>33150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>36000</v>
+      </c>
+      <c r="C8">
+        <v>58320</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A5:C8">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A5))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:C8">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>